<commit_message>
Add missing constraints to scrnaseq (#652)
* Copy over missing constraints from atacseq

* regen

* changelog

* Required field; regen
</commit_message>
<xml_diff>
--- a/docs/scrnaseq/scrnaseq-metadata.xlsx
+++ b/docs/scrnaseq/scrnaseq-metadata.xlsx
@@ -12,7 +12,10 @@
     <sheet name="assay_category list" sheetId="3" r:id="rId3"/>
     <sheet name="assay_type list" sheetId="4" r:id="rId4"/>
     <sheet name="analyte_class list" sheetId="5" r:id="rId5"/>
-    <sheet name="library_final_yield_unit list" sheetId="6" r:id="rId6"/>
+    <sheet name="sc_isolation_entity list" sheetId="6" r:id="rId6"/>
+    <sheet name="sc_isolation_enrichment list" sheetId="7" r:id="rId7"/>
+    <sheet name="library_layout list" sheetId="8" r:id="rId8"/>
+    <sheet name="library_final_yield_unit list" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -588,7 +591,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>version</t>
   </si>
@@ -668,12 +671,30 @@
     <t>sc_isolation_entity</t>
   </si>
   <si>
+    <t>whole cell</t>
+  </si>
+  <si>
+    <t>nucleus</t>
+  </si>
+  <si>
+    <t>cell-cell multimer</t>
+  </si>
+  <si>
+    <t>spatially encoded cell barcoding</t>
+  </si>
+  <si>
     <t>sc_isolation_tissue_dissociation</t>
   </si>
   <si>
     <t>sc_isolation_enrichment</t>
   </si>
   <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>FACS</t>
+  </si>
+  <si>
     <t>sc_isolation_quality_metric</t>
   </si>
   <si>
@@ -690,6 +711,12 @@
   </si>
   <si>
     <t>library_layout</t>
+  </si>
+  <si>
+    <t>single-end</t>
+  </si>
+  <si>
+    <t>paired-end</t>
   </si>
   <si>
     <t>library_adapter_sequence</t>
@@ -1157,83 +1184,83 @@
         <v>25</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="10">
+  <dataValidations count="15">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
       <formula1>'version list'!$A$1:$A$1</formula1>
     </dataValidation>
@@ -1249,8 +1276,25 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="N2:N1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: whole cell / nucleus / cell-cell multimer / spatially encoded cell barcoding." sqref="R2:R1048576">
+      <formula1>'sc_isolation_entity list'!$A$1:$A$4</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: none / FACS." sqref="T2:T1048576">
+      <formula1>'sc_isolation_enrichment list'!$A$1:$A$2</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: single-end / paired-end." sqref="Z2:Z1048576">
+      <formula1>'library_layout list'!$A$1:$A$2</formula1>
+    </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="AC2:AC1048576">
       <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="AG2:AG1048576">
+      <formula1>-2147483647</formula1>
+      <formula2>2147483647</formula2>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="AH2:AH1048576">
+      <formula1>-2147483647</formula1>
+      <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AI2:AI1048576">
       <formula1>-1e+307</formula1>
@@ -1367,6 +1411,85 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1375,7 +1498,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
distinguish v2 and v3 10x
</commit_message>
<xml_diff>
--- a/docs/scrnaseq/scrnaseq-metadata.xlsx
+++ b/docs/scrnaseq/scrnaseq-metadata.xlsx
@@ -591,7 +591,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>version</t>
   </si>
@@ -635,7 +635,10 @@
     <t>assay_type</t>
   </si>
   <si>
-    <t>scRNAseq-10xGenomics</t>
+    <t>scRNAseq-10xGenomics-v2</t>
+  </si>
+  <si>
+    <t>scRNAseq-10xGenomics-v3</t>
   </si>
   <si>
     <t>scRNAseq</t>
@@ -1166,97 +1169,97 @@
         <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1267,8 +1270,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: sequence." sqref="K2:K1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: scRNAseq-10xGenomics / scRNAseq / sciRNAseq / snRNAseq / SNARE2-RNAseq." sqref="L2:L1048576">
-      <formula1>'assay_type list'!$A$1:$A$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from assay_type list." sqref="L2:L1048576">
+      <formula1>'assay_type list'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: RNA." sqref="M2:M1048576">
       <formula1>'analyte_class list'!$A$1:$A$1</formula1>
@@ -1355,7 +1358,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1384,6 +1387,11 @@
     <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1401,7 +1409,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1419,22 +1427,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1452,12 +1460,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1475,12 +1483,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1498,7 +1506,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add new field and regen
</commit_message>
<xml_diff>
--- a/docs/scrnaseq/scrnaseq-metadata.xlsx
+++ b/docs/scrnaseq/scrnaseq-metadata.xlsx
@@ -452,11 +452,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>Parameter for downstream pipeline; How many cells are expected?</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AH1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Number of PCR cycles to amplify cDNA</t>
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0">
+    <comment ref="AI1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -469,7 +482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0">
+    <comment ref="AJ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -482,7 +495,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0">
+    <comment ref="AK1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -495,7 +508,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0">
+    <comment ref="AL1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -508,7 +521,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0">
+    <comment ref="AM1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -521,7 +534,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0">
+    <comment ref="AN1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -534,7 +547,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0">
+    <comment ref="AO1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -547,7 +560,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO1" authorId="0">
+    <comment ref="AP1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -560,7 +573,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP1" authorId="0">
+    <comment ref="AQ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -573,7 +586,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ1" authorId="0">
+    <comment ref="AR1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -591,7 +604,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>version</t>
   </si>
@@ -735,6 +748,9 @@
   </si>
   <si>
     <t>cell_barcode_size</t>
+  </si>
+  <si>
+    <t>expected_cell_count</t>
   </si>
   <si>
     <t>library_pcr_cycles</t>
@@ -1119,7 +1135,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AQ1"/>
+  <dimension ref="A1:AR1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1128,7 +1144,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:44">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1238,7 +1254,7 @@
         <v>51</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AL1" s="1" t="s">
         <v>54</v>
@@ -1258,9 +1274,12 @@
       <c r="AQ1" s="1" t="s">
         <v>59</v>
       </c>
+      <c r="AR1" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="15">
+  <dataValidations count="16">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
       <formula1>'version list'!$A$1:$A$1</formula1>
     </dataValidation>
@@ -1296,18 +1315,22 @@
       <formula1>-2147483647</formula1>
       <formula2>2147483647</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AI2:AI1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="AI2:AI1048576">
+      <formula1>-2147483647</formula1>
+      <formula2>2147483647</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AJ2:AJ1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: ng." sqref="AJ2:AJ1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: ng." sqref="AK2:AK1048576">
       <formula1>'library_final_yield_unit list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AN2:AN1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AO2:AO1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AO2:AO1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AP2:AP1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
@@ -1498,7 +1521,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
distinguish v2 and v3 10x (#661)
</commit_message>
<xml_diff>
--- a/docs/scrnaseq/scrnaseq-metadata.xlsx
+++ b/docs/scrnaseq/scrnaseq-metadata.xlsx
@@ -591,7 +591,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
   <si>
     <t>version</t>
   </si>
@@ -635,7 +635,10 @@
     <t>assay_type</t>
   </si>
   <si>
-    <t>scRNAseq-10xGenomics</t>
+    <t>scRNAseq-10xGenomics-v2</t>
+  </si>
+  <si>
+    <t>scRNAseq-10xGenomics-v3</t>
   </si>
   <si>
     <t>scRNAseq</t>
@@ -1166,97 +1169,97 @@
         <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1267,8 +1270,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: sequence." sqref="K2:K1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: scRNAseq-10xGenomics / scRNAseq / sciRNAseq / snRNAseq / SNARE2-RNAseq." sqref="L2:L1048576">
-      <formula1>'assay_type list'!$A$1:$A$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from assay_type list." sqref="L2:L1048576">
+      <formula1>'assay_type list'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: RNA." sqref="M2:M1048576">
       <formula1>'analyte_class list'!$A$1:$A$1</formula1>
@@ -1355,7 +1358,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1384,6 +1387,11 @@
     <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1401,7 +1409,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1419,22 +1427,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1452,12 +1460,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1475,12 +1483,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1498,7 +1506,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Apply to v2 instead of v1 of the schema
</commit_message>
<xml_diff>
--- a/docs/scrnaseq/scrnaseq-metadata.xlsx
+++ b/docs/scrnaseq/scrnaseq-metadata.xlsx
@@ -604,7 +604,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>version</t>
   </si>
@@ -648,7 +648,10 @@
     <t>assay_type</t>
   </si>
   <si>
-    <t>scRNAseq-10xGenomics</t>
+    <t>scRNAseq-10xGenomics-v2</t>
+  </si>
+  <si>
+    <t>scRNAseq-10xGenomics-v3</t>
   </si>
   <si>
     <t>scRNAseq</t>
@@ -1182,100 +1185,100 @@
         <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1286,8 +1289,8 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: sequence." sqref="K2:K1048576">
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: scRNAseq-10xGenomics / scRNAseq / sciRNAseq / snRNAseq / SNARE2-RNAseq." sqref="L2:L1048576">
-      <formula1>'assay_type list'!$A$1:$A$5</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from assay_type list." sqref="L2:L1048576">
+      <formula1>'assay_type list'!$A$1:$A$6</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: RNA." sqref="M2:M1048576">
       <formula1>'analyte_class list'!$A$1:$A$1</formula1>
@@ -1378,7 +1381,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1407,6 +1410,11 @@
     <row r="5" spans="1:1">
       <c r="A5" t="s">
         <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1424,7 +1432,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1442,22 +1450,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -1475,12 +1483,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1498,12 +1506,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1521,7 +1529,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mccalluc/expected cell count (#668)
* New version, but no real changes

* regen

* Add new field and regen

* More regen

* changelog

* Suggestions from Matt

* regen

* Apply to v2 instead of v1 of the schema
</commit_message>
<xml_diff>
--- a/docs/scrnaseq/scrnaseq-metadata.xlsx
+++ b/docs/scrnaseq/scrnaseq-metadata.xlsx
@@ -452,11 +452,24 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
+          <t>How many cells are expected? This may be used in downstream pipelines to guide selection of cell barcodes or segmentation parameters.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AH1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
           <t>Number of PCR cycles to amplify cDNA</t>
         </r>
       </text>
     </comment>
-    <comment ref="AH1" authorId="0">
+    <comment ref="AI1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -469,7 +482,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AI1" authorId="0">
+    <comment ref="AJ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -482,7 +495,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AJ1" authorId="0">
+    <comment ref="AK1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -495,7 +508,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AK1" authorId="0">
+    <comment ref="AL1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -508,7 +521,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AL1" authorId="0">
+    <comment ref="AM1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -521,7 +534,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AM1" authorId="0">
+    <comment ref="AN1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -534,7 +547,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AN1" authorId="0">
+    <comment ref="AO1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -547,7 +560,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AO1" authorId="0">
+    <comment ref="AP1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -560,7 +573,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP1" authorId="0">
+    <comment ref="AQ1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -573,7 +586,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ1" authorId="0">
+    <comment ref="AR1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -591,7 +604,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>version</t>
   </si>
@@ -738,6 +751,9 @@
   </si>
   <si>
     <t>cell_barcode_size</t>
+  </si>
+  <si>
+    <t>expected_cell_count</t>
   </si>
   <si>
     <t>library_pcr_cycles</t>
@@ -1122,7 +1138,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AQ1"/>
+  <dimension ref="A1:AR1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1131,7 +1147,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:43">
+    <row r="1" spans="1:44">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1241,7 +1257,7 @@
         <v>52</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="AL1" s="1" t="s">
         <v>55</v>
@@ -1261,9 +1277,12 @@
       <c r="AQ1" s="1" t="s">
         <v>60</v>
       </c>
+      <c r="AR1" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="15">
+  <dataValidations count="16">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
       <formula1>'version list'!$A$1:$A$1</formula1>
     </dataValidation>
@@ -1299,18 +1318,22 @@
       <formula1>-2147483647</formula1>
       <formula2>2147483647</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AI2:AI1048576">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="AI2:AI1048576">
+      <formula1>-2147483647</formula1>
+      <formula2>2147483647</formula2>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AJ2:AJ1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: ng." sqref="AJ2:AJ1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: ng." sqref="AK2:AK1048576">
       <formula1>'library_final_yield_unit list'!$A$1:$A$1</formula1>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AN2:AN1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AO2:AO1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
-    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AO2:AO1048576">
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a number" error="The values in this column must be numbers." sqref="AP2:AP1048576">
       <formula1>-1e+307</formula1>
       <formula2>1e+307</formula2>
     </dataValidation>
@@ -1506,7 +1529,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
... and the fix
</commit_message>
<xml_diff>
--- a/docs/scrnaseq/scrnaseq-metadata.xlsx
+++ b/docs/scrnaseq/scrnaseq-metadata.xlsx
@@ -609,7 +609,7 @@
     <t>version</t>
   </si>
   <si>
-    <t>1</t>
+    <t>2</t>
   </si>
   <si>
     <t>description</t>
@@ -1283,7 +1283,7 @@
     </row>
   </sheetData>
   <dataValidations count="16">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 1." sqref="A2:A1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 2." sqref="A2:A1048576">
       <formula1>'version list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: sequence." sqref="K2:K1048576">

</xml_diff>

<commit_message>
back to int; regen
</commit_message>
<xml_diff>
--- a/docs/scrnaseq/scrnaseq-metadata.xlsx
+++ b/docs/scrnaseq/scrnaseq-metadata.xlsx
@@ -439,7 +439,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Position(s) in the read at which the umi barcode starts.</t>
+          <t>Position in the read at which the umi barcode starts.</t>
         </r>
       </text>
     </comment>
@@ -1339,7 +1339,7 @@
       </c>
     </row>
   </sheetData>
-  <dataValidations count="20">
+  <dataValidations count="21">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: 3." sqref="A2:A1048576">
       <formula1>'version list'!$A$1:$A$1</formula1>
     </dataValidation>
@@ -1374,6 +1374,10 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not a boolean" error="The values in this column must be &quot;TRUE&quot; or &quot;FALSE&quot;." sqref="AC2:AC1048576">
       <formula1>"TRUE,FALSE"</formula1>
+    </dataValidation>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="AF2:AF1048576">
+      <formula1>-2147483647</formula1>
+      <formula2>2147483647</formula2>
     </dataValidation>
     <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Not an integer" error="The values in this column must be integers." sqref="AG2:AG1048576">
       <formula1>-2147483647</formula1>

</xml_diff>

<commit_message>
snRNAseq-10xGenomics-v3 was missing from the scRNAseq assay lists (#1050)
* snRNAseq-10xGenomics-v3 was missing from the scRNAseq assay lists

* update_yamls to fix CI

* update docs/field-assays.yaml

* update docs/scrnaseq

* changelog

Co-authored-by: mccalluc <mccalluc@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/docs/scrnaseq/scrnaseq-metadata.xlsx
+++ b/docs/scrnaseq/scrnaseq-metadata.xlsx
@@ -643,7 +643,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
   <si>
     <t>version</t>
   </si>
@@ -694,6 +694,9 @@
   </si>
   <si>
     <t>snRNAseq-10xGenomics-v2</t>
+  </si>
+  <si>
+    <t>snRNAseq-10xGenomics-v3</t>
   </si>
   <si>
     <t>scRNAseq</t>
@@ -1236,109 +1239,109 @@
         <v>13</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="AF1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="AG1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="AH1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AI1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="AJ1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="AK1" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="AL1" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="AM1" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="AN1" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="AO1" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="AP1" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="AQ1" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AR1" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="AS1" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="AT1" s="1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="AU1" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1350,7 +1353,7 @@
       <formula1>'assay_category list'!$A$1:$A$1</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must come from assay_type list." sqref="L2:L1048576">
-      <formula1>'assay_type list'!$A$1:$A$7</formula1>
+      <formula1>'assay_type list'!$A$1:$A$8</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Value must come from list" error="Value must be one of: RNA." sqref="M2:M1048576">
       <formula1>'analyte_class list'!$A$1:$A$1</formula1>
@@ -1461,7 +1464,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1500,6 +1503,11 @@
     <row r="7" spans="1:1">
       <c r="A7" t="s">
         <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -1517,7 +1525,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -1535,22 +1543,22 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1568,12 +1576,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1591,12 +1599,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1614,7 +1622,7 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>